<commit_message>
Day 3 part 2
</commit_message>
<xml_diff>
--- a/Felix/Day3/24d3p1.xlsx
+++ b/Felix/Day3/24d3p1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nmca-my.sharepoint.com/personal/felix_french_mail_nidec_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b58bf48a7331aef/Documents/AdventOfCode/aoc24/Felix/Day3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{D88EDA5B-D22C-4AEF-BED0-8719F3FDB82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4F0C064-9857-4102-B661-C38AAC9E3F95}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{D88EDA5B-D22C-4AEF-BED0-8719F3FDB82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97022B1A-DBD4-416A-A560-864CBC6BBB95}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9BC4DD3-9E69-4E94-82BB-889EE700334F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -85,15 +85,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>find ,</t>
+    <t xml:space="preserve"> (who() what())&gt;when()why()'mul(454,153)mul(565,994)(mul(890,533)#mul(875,768)+'-^where()}when()mul(103,598)[mul(401,600)when()from()how()+mul(928,225)why():mul(909,344)when()'?where():(what()mul(972,219)${/ mul(402,908)who()&amp;where()~where()mul(60,961)#]$mul(459,473))})~mul(143,89),select()mul(772,463)mul(742,92)&lt;(]},select()[%^when()don't()select()from()mul(776,917)+!!why()when(485,399)what(720,754)from()&amp;mul(746,260)where()*who()~&amp;/from()what()]what()mul(694,820)%why(16,195)when()'why() [when()why():do()when(),'&lt;?{who()mul(296,514)%mul(442,333)when()-,why()[!:+from()mul(774,695)}where()*-!%mul(834,493){-&amp;(??mul(240,739)from()@@}@mul(796,837)[;mul(301,618)mul(933,68)+%}/$&lt;mul(879,769)'&amp;('#-mul(314,537);who()where(134,686) where(975,359){how(900,557)mul(134,21)when() !*!$^mul(670,298)*!}:-how(429,820)~]mul(414,322)-select()?what()when()]&gt;#from()(mul(200,440)/]mul(58,834)@&lt;select()mul(966,435)&lt;+;mul(98,983)&lt;;,;how()&amp;'@mul(727,703)!?&gt;!!mul(175,542)mul(363,28)]}don't()+[{&lt;@/,mul(103,154)mul(808,942)$where()why()from()[mul(780,395)^why()#-!:~why()+mul(879,633)&lt;[where()!what()-,mul(6,80)how()?)^select()&lt;}when()]how()mul(385,345)~?don't()&lt;)'mul(557,404)+;/&lt;;}%?//mul(586,270);^&amp;,^}'&amp;:mul(914,485)&gt;,$mul(616,138)'[/-mul(786,357)&amp;why()where(490,893)/-}*}mul(967,485)!'mul(664,982),when()^why()$%(,why()mul(826,970)$*~'),+when()-mul(586,837)+;(/%{[what(201,897)mul(540,583)don't()}mul(358,207)mul(988,94)$#&amp;&lt;?+why()mul(82,18):from()select()!~mul(805,768)&amp;+! how()what()?select())mul(779,277)[&gt;}mul(580,42)#select(190,243){*%*from()mul(491,435)* mul(345,720)+#{)/,'&lt;},mul(529,664)? don't()'mul(925,474)}:!?]mul(655,353)when()'how()(don't()how()^/where())select()select()^~{mul(39,73)['[&lt;^)/!;&lt;mul(367,290)$select()when()^when()&gt;mul(338,323) ~* who()what()where()mul(746,703)mul(70,40);/&lt;select()mul(557,879)*&gt;:!mul(89,464)when()how()~?;~}mul(669,359)+mul(64,989)why()what()where(478,19)^from()$mul(49,43):why()mul(946,368)who()%?{'why()mul(754,618)select()}^mul(925,787)how()select()&lt;^;{}}%mul(857,178)@?$;)%what()['mul(343[&lt;^mul(622,524)$#{&amp;where();@how() #mul(572,8)who(244,369)/*;;mul(22,910)how()?who(200,683)#what()why()mul(9,541)don't() %&gt;mul(583,678)mul(977,618)mul(846,566):@mul(601,58)%mul(12,677)^#[how()?do()&amp;'%how(985,614);@? 'mul(295,467)}@mul(462,179)[from(946,303)@what(236,293),from(572,15)^mul(602,286/*:(select()!mul(950,26){^}]-mul(541,949){/select() from(202,590)what()]select()~mul(931,833)^/}where()*mul(665,272)*'where()&gt;} :]mul(470,26))mul(945,496)%-!;-* mul(958,735)+mul(292,844)where()mul(323,887)select()how()why()%~why(974,789){!/:mul(890,844)&amp;]{'mul(727,812)?mul(521,348)']~,mul(604#what(201,469)]{'how()#[mul(68,187){#+%* when()+when()mul(270,65)select())how();! %where()]@mul(267,348)from()select()who(579,714)where()mul(359,887why()who(120,403)from()&amp;!)do()mul(614,872)select()[:who()'&gt;&gt;?]who()mul(373!:&gt;&amp;mul(13,848)~how()who()+*what()&amp;mul(214,262)/where(941,723)mul(34,526){ }( ~from()){ mul(648,400)mul(946,270)where()&lt;mul(672,282)&amp;'&gt;,mul(156,431)when(444,909)mul(10,765)#mul(393,855)how()@&amp;from()mul(538,109)[%^-&lt;(how()}how()mul(841,917)~ ]^! ^select()mul(624,87))what()&amp;[-'/&amp;)mul(113+from()how()why()]&amp;&gt;mul(82,319)&amp;:''where()/&lt;;mul(882,75)&gt;/^#/how()!mul(481,243)}*!what()#}#mul(93,825)&gt;'(!where()(&amp;mul(417,293)&gt;[{*()}how(349,243))mul(577,515)}mul(644,588)why()~~what()'why(658,231)]where()mul(260,870)mul(82,64)$+&gt;,&amp;$where()$why()where()mul(513,597),when()why()&amp;mul(559,679/why();~{mul(876,302)/+why(921,489);%@from(){do()&amp;+from()mul(646,666)how() }^;{!?mul?),$*mul(244,591)&lt;)select()(&lt;where()(!mul(708,996)/*@;;:mul(760,261)when(338,104)mul(870,299)!}(mul(269,625) who(553,681)&amp;mul}[#{who()%what(){,when()mul(723,486)-/?{mul(475,745)&amp;%select()%'who()&lt;?:mul(117,765):{&gt;^select()where(454,602)when(){mul(201,421)) ,when()$/$;#;mul(715,512)~-mul(110select())&amp;/;&gt;:^')+mul(525,861)mul(94,520)select();mul(200,362)mul(662,110)what()[';mul(706,110)mul(524,196{ from()%/from()when()select()*mul(952,760)@&lt;@(mul(359,289:?[!:mul(788,331)&gt;(-mul(790,172)~/';(#mul(744,504)}@!#:!)where()mul!why()&lt;+mul(24,595)($/why()&amp;(&lt;mul(872,460%where()[who()mul(962,669):&lt;+-from()]mul(454,164)-,what()@+'mul(10,853)-@@){}what()mul(909,997) ^why()@!/from()$]mul(97,897)?mul(935,220)why()[:*)^) #/mul(301,584)@where()how()mul(609,313)':mul(949from();who())who()who()mul(491,372)!&gt;&gt;'why()}/mul(809,414)mul(202,168)&amp; where(){- ]where()where()&lt;mul(281,296);&amp;mul(625,586)!/{]&amp;+&gt;who()&gt;^mul(543,106){don't():/('why()when()[):#mul(261,544)why()-+mul(325,976)-why()&amp; what()who()%*&amp;;mul(309,586)from()~;mul(527,332)]how()when()mul(266,71)mul(383,68)how()from()}how()[{;who()why()mul(479,649)-who()&gt;mul(954,835))(,'?)why(),mul(73,982)-+mul(275,963)?:*&gt;+%%}%mul(159,868)[{mul(849,590)where()how()when()mul(380,542),'{mul(716,261)@$what()[where(961,898)+#;mul(102,332))mul(151,993)who(433,641)what()!],{&lt;why()#mul(449,110)?from()~how()how()how(425,48)where()~mulwhen()mul(427,877)when()+!&lt;who(),&gt;}mul(225,989)from()$&gt;'/&gt;mul(271,482)(]when(703,790)$['&amp;don't()^ mul(292,747)why();;from()why() #[??mul(675,831)*/&lt;{when()%mul(82,353)?~(~@from()-mul/,when()[+', /why()mul(531,95)')&lt;&amp;#]#!&lt;mul(172,129)mul(543,657-[&lt;,:,:@mul(458,222)mul(640,872)^mul(45,292)!&amp;#+mul(859,346)[:+^$how()(&lt;when()mul(247,266)mul(468,925)&amp;select()^who()~))mul(184,981)from() when()+select()&gt;where()&lt;when()mul(420,131)+-select(379,472)-$from())mul(402,68)what()#mul(278,846)#who()~)?mul(287,731)-- mul(989,728)#$when():mul(470,964why()$ )-?,':from()from()mul(54,842)}mul(581,400),{$select()select()how()mul(531##mul(272,787)['{(don't(),[how()?@where()@-^-mul(55,325)#,][?mul(437,664)+-select()what():/%'mul(569,297))'?/*{mul(40,581)^how()where()!who()#[mul(828,836)$why(819,535)who()#/&gt;$&gt;select()[mul(326,511)/:#::when()(do();mul(960,765$mul(947,618)!from(704,544)-);select()}mul(278,843)&amp;+-&amp;)!}select()why()mul(333,183)!~mul(360,636)}@mul(43,235)&amp; ~*how()~&amp;&gt;$~mul(163,420);@' mul(328,120)&amp;}#)what()~[~!mul(892,685);from())*select()]from(),mul(454,194)!what(598,913)~what()who()*),*who()mul(651,343)~'mul(311,104)~%~how(){when(){mul(348,414)!who()when(),mul(565,187)'who()mul(573,606)/]&lt;why())mul(29,128)%from()select();]where()'%mul(515,513):'why()/&lt;&amp;#%-mul(54,420)what()mul(253,192)}how()+mul(344,599[$who()#what()@from(850,461)mul(670,417)why()!mul(77,694)who()::+who()(^mul(580,475)(&gt;/?^{do()when(),mul(301,391)select()!]%mul(662,532)why():&gt;mul(317,266)-]/!#?~what(395,165)mul(882,259)(how(){%)from(355,754)from(){?+mul(251,179)+}$^-[mul(244,700), $$mul(989,641)how()&amp;&gt;[{(@when()!mul(17,250)why()mul(516,948)/from()&amp;)](~who(),mul(936,726)from()who()mul(642,108){?/*&lt;mul(421,307) mul(954,385)@-who()-]why()do()mul(152,214)?)what()what() ){select()/mul(88,987)(&amp;;^where(687,768)mul(592,288)&gt;:who()](-)[mul(234,936)//select(){don't()}!mul(711,979)when()why()~( what()%from()^:mul(970,839)who()~$from()how()mul(525,184)(*}from())mul(592,712)select()where()from()do()/!from()@%* /:mul(796,770)[select()mul(737,95)*who()mul(538,295)from()when()mul(202,997)mul(920,622)[^,'^{~&amp;mul(890,310)-#mul##$what()how(),*{]what()'mul(753,51)why()from()%+*-mul(44,560)^/who() how()mul(846,745),$ mul(884,965)?];@;'mul(607,810)]don't()?mul(15,474)*^%where()&gt;,#- mul(381,876)&gt;]'how()[]?when()mul(350,528)&amp;&gt;%%#*;mul(465,783)?/from()'mul(109,659)*'mul(260,549))where(427,3)mul(750,184)mul(514,568)+ &lt;mul(142,867)do(){ mul(197,631)*[~![mul(592,975)&gt;where(838,713) ~$]{what()mul(505,954)&lt;&gt;;-#:mulwhat()[!]why()mul(899,266)%}&gt;select()?]'mul(936,764),~mul(189,689)}^mul(474,190)&lt;;&amp;&gt;]how()/{mul(271,843)&gt;}why(522,791)what()do()#/^where()%when()!mul(284,340)##[why() when()&gt;{mul(998,539)*[*):'&gt;'mul(577,914)[*)who()mul(305,505)who()!@how()'}when()mul(331,543))mul(91,478)(where(196,348)&amp;:]&gt;?mul(560,724)where(872,560)&lt;% what()*where()]select()do()(what()-~mul(229,896){?~when()mul(826,622)&amp;(#mul(451,442))what()mul(866,906)how()$-&amp;where()&gt;-([mul(199,824)!~)$/&lt;:mul(727,123)do()$*-#-@+where()select()$mul(612,415)who()$#,who()&gt;/from()mul(967*who();%@}how()/why()}mul(106,998)how():(;&amp;mul(345,702)mul(275,94)]#&gt;{mul(426,479)why()&lt;;~what()$!+@'mul(40,71)&amp;when()*%mul(973,215),what(),mul(709,788)who()):mul(205,236)~mul(50,81)+how()%~/mul(748,800)(}}mul(124,528)mul(129,959)%[&amp;[select()mul(547,292);who()&gt;???why()+who()mul(442,582):how()&gt;select(92,760);+mul(440,501)@/@&gt;#&amp;:mul(764,753select()%:how()where(202,288) mul(613,367)how()?mulselect(255,7);[;why()/$ mul(351,228){mul(312]+!^#+,why()what(327,951)mul(134,668)&amp;&lt;why(575,717) $-('mul(810,445),mul(731,60)^:mul(695,596)~*^;/mul(570,879)why()where()where() select()what();(from()&lt;mul(11~what()select()how()$-&lt;%mul(335,108)~[)mul(759,937)mul(93,397)when()&gt;&amp;?'!why()where()mul(172,288)+mul(90,27):';*@how()/what()mul(272,960)select(845,387)don't()&lt;select(142,144)how(){}mul(525,125)mul(513,731)from()@,@}why():;:don't()+why()mul(758,764)@,:mul(248,570)/!mul(352,81)what()/?&lt;::what(),}^mul(723,61)'$'^don't()!-from()$**^mul(340,35)where()why(16,588):-mul(895,416)$how()!where()'~{'+,mul@where()&lt;(who():&lt;mul(857,771)}mul(231 when())+mul(494,721)#!/usr/bin/perlmul(361,116)(^*mul(552,797)mul(235,864)[%@~}~mul(222,585))where()where()/{^#@mul(3,798)what()what()where()why()#how()&amp;mul(607!who()+select()what(315,999)/mul(322,478)'when(),why(885,556)select(747,859)^}how()#mul(994,4)what()&lt;/(mul(534,885)who())};from()why()}from()~what()mul(858,35!:why()what()what()mul(716,993)why()&gt;}--}}?)mul(509,779)-)mul(682,498))from()#mul(69,525)%-?&gt;&gt;mul(68,359)/mul(923,989from()~mul(132,353)mul(980,998) (where()}*&gt;&amp;how()[mul(570,289)*~mul(388,859)how(829,278)[&lt;]who();&lt;who()[mul(833,723;mul(208,875)&gt;mul(199,174)*~:[what()^}#who()&gt;mul(221,636)*-()%-when()from()mul&amp;}who()[mul(725,983)&gt;#!who(592,5)%mul(85,978)what()'mul(178,305)[[?:#-&gt;#! mul(374,804)&lt;$&amp;{-&gt;++mul(446,37)-#&amp;}%)mul(19,914who()(# ;mul(959,330)what()&gt;#who()who();mul(228,273)from()+}/&amp;why(783,754)from()(#mul(649,849)*why(){why()(who()?!why()from()mul(344,447):how()+when(144,750)what()mul(217,542)where())%mul(253,8),$how()%[&gt;#from(),:mul(174,127)-:when()-don't()where()(when()&amp; ]^from()mul(263,164)mul(873,530)::@select()mul(459,547)why()!}$*mul(674,506)&lt;mul(665,313)@mul(310,284)when()how()#;+({@~mul(655,423)(?where(868,382)where()@mul(190,467))-when()~how()mul(71,646)where()how() mul(362,510)&gt;*]~don't()mul(570,150)what()do()&lt;'^)~mul$mul(508,426)/why()mul(155,774)~?from()![mul(670,674)select()?^when()from()]{mul(736,574){&gt;'~^mul(248,37where()@:where(938,730)select()!'&gt;,;mul(827,796):what()%where()!/how(231,307)mul(88,489)@!!mul(173,890)how()[- +what()+$~mul(244,436)(why(),[,-;[&lt;%mul(991,950)%mul(804,561)&amp;:,mul(442,575)}~what(523,563)?+ how()/}[mul(866,343)]:where()where()&gt;$mul(423,440)~&gt;[mul(259,864))@ {^mul(256,238)[:]*$$mul(206,916)*}!what(937,263)select()}don't()'*&amp;mul(630,249),mul(521,101)&lt;where()?where()how()from()select()&lt;when():mul(185,154)$*&lt;(do()]{mul(231,307)$*@* why()select()%'@mul(564,503)@ !@mul(245,476)who()how()$@~select()&gt;/who()!mul(884%/&amp;;^from()mul(846,533);}why()?;mul(538,765)+,([ !}@]{mul(98,545) ~how(703,291)]#)~[[mul(588,167)*-+mul(246,51);+from(){;;what()/:?mul(921,460)&lt;@where()mul(674,502)/)select()%~what()?)mul(406,916)&gt;/mul(501,656)]mul(979,533)/why()*select()where(),^mul(370,549)^~how()why()+,how()@mul(168,884)',&lt;$]mul(377,183)+$&lt;mul(48,619)who(625,236)who()#where()}mul(43,845)why()(?~mul(575,269)&amp;who()why()(!where()-]mul(482,691)where(745,121)from()^/{mul(784,137)@where()(#do():-%]''{mul(901,539)/@who()%&lt;mul(979,206)mul(705,493))&gt;mul(425,602)when()~'&gt;when(),when()%mul(231,25)[why();'!mul(879,941/who()mul(658,479)why()where()*mulwhen()mul(486,551)where()?,)~ what(221,542)/;mul(260*how()~~why()mul(571,395)mul(319,33)where()mul(313,612)select(458,89)when()?from(),)[%^[mul(489,554){mul(482,42)from();mul(911,838)from()what()&amp;/when()when()mul(748,509)/!&amp;who()mul(98,104)what()',how(660,701)^mul(904,678)&amp;}'mul(498,173select()% -from()!when()mul(918,395)?&lt;&lt;@mulhow()/from()][don't()+select()who()what():^^@mul(826,867)select()^[@mul(673,493)select()@(select()mul(152,937),why(955,595)select()where()-'mulwhere()~?mul(572,408)when(606,22){~*(mul(971,805),how(402,696)')}who()&amp;@*who()mul(76,96){where()mul(711,3)*-+~where()mul(812,534[select()!#(how()mul(799,474)&gt;mul(251,649)(from()what();-do()~;]what(),what(393,86)?mul(892,224)who()mul(635,260)mul(300,39)}&gt;select()&gt;@why(364,672)who():where()mul(385who()))&gt;when()why()&amp;&gt;mul(276,702)&amp;:mul(192,782)/:)@mul(948,155)[!don't())what(),what()mul(747,717)#?$mul(967,489)when()who()why()#mul(961,811)what()mul(307,623)~}from()how(),mul(669,93)^ &amp;select()how()mul(105,129)?])*)mul(246,433):)how()mul(941,140)&lt;[ ;&amp;*mul(580,48);%%'why()what()( %mul(189,229)]'&lt;@)/mul(741,684)[mul(632,558)'@what()what()mul(986,227)&lt;how(584,802)$mul(698)@;+%+;mul(704,986){{how()where()what()from()where()$do()where()why()*-mul(752,877);where()//*?*&gt;&lt;?mul(33,338)where()where()[&gt;select()/from()*when()@mul(747,356)mul(674,720)mul(10,513))]#]-mulwhat()select(501,639)mul(114,558)[}$]who()mul(759,134)#who()/@*mul(444,475)!@+don't()#when()}where()[where()',select(){mul(206,80)/&lt;what(230,519)-mul(424,213)&gt;!&amp;how()+]^mul(847,293)+(mul(837,220)/!#!mul(613,470)&lt;mul(93,129)who()from()&gt;#where()from()&amp;$mul(29,370how()]&amp;&lt;where()from(283,113)mul(336,151)select();-from()'why()when()how()(what()mul(467,47){{??mul(513,543);)mul(397,402)mul(428,472)who()~{mul(262,609)how()from(){'  /who()select()mul(778,88)~&gt;/-where()%from())&gt; mul(251,617)-why()~^don't()##~mul(176,935)[;%@?^,don't()!mul(564,493-(&amp;+@'[&lt;*;mul(241,470)&lt;&gt;}mul(684,534):?&lt;do()mul(336,113)&gt;[&gt;?+:mul(835,881)mul(901,992)mul(595,306what()% mul(333,684),what(910,959);^what(),where()'mul(493,314)}-what()&amp;who(231,428)where()&gt;' &lt;mul(754,558)how()+what(734,212)]how()$)^mul(991,39))-'}{mul(459,367);@^-?]?$?mul(32,624)how())mul(741,402)*@]when()mul(559,247)when()don't()((,[}-why(692,780)({{mul(788,419)how() -)mul(710,838)mul(952,75)/!#')[([&lt;mul(547,553)(@&lt;!~]#+who()+mul(597,266)&gt;[where(),]who()mul(215,607)&amp;'mul}select()^%&lt;!mul(523,490);';)(@}&gt;/what()do()&amp;mul(735,766)#%$']*;/+do()~what()how();$#[/select()mul(73,86),who()#who()?*&lt;mul(285,423)'@don't()-!$};where()^%mul(846,592)mul(129,272)[)&lt;when()&gt;[mul(839,173)&amp;$$[why(349,377){why()&gt;why()mul(49,44)@'};!)*;mul(265,467)why()}'mul(561,416)}]-mul(334,113)mul(126,247)}mul(536,247){?mul(780,762)&lt;from()~-] @+$mul(416,370)$mul(617,551)who(647,22){&lt;':}!when()how()mul(541#what())~select()where(257,55)?when(446,792)mul(654,34)mul(30,36)^+'}*mul(835,84};)mul(348,922)who()what(424,481))$(!@^[mul(934,712[&gt;,how()&lt;'who()what()%&lt;?mul(909,44)how()~(do()[&lt;]+[mul(30,114)select()where()[&gt;what()mul(324,650)* ^)mul(116,480)&amp;  %&gt;,mul(722,539)-who()mul(69,643))+select()&lt;'mul(398,585)mul(635,160),!{}mul(218,149))(why()[when(),mul(4,152)@what()*@&gt;@how()mul(78,645)@*#}#select()({mul(196,97)when()@what()+why(287,586)when(){mul(908,484{%-where(){'from()mul(254,416)how()}*(how()#@}mul(670,932)mul(741,232)&amp;'!?@$mul(775,804);),,!mul(757,128)/?'!mul(47,297) $/,,:@~select()?mul(604,497);mul(770,711)+mul?where()/mul(777,175)^&gt;where()&lt;#mul(376,176)~){}mul(758,497)!){%where(), mul(360,122,mul(54,973)):mul(248,44)[where()^mul(162,809))*what()^?+}what()how()why()mul(839,131)mul(913,94) why(),why()'mul(459,43)&lt;-from(),#%{]%/mul(733,345){,/+&lt;[?mul(292,416)&amp; [&gt;/^why(408,559)mul(648,879)#)$ +how()where()#mul(708,178)how()*[mul(560,727)*when()from(); &gt;~]'&amp;mul(90,393)$~from()mul(578,828)mul(710,50)?+@what()@+!;mul(250,79)when())'mul(523,730)+*}^*mul(698,766)&lt;-why()-/:!/select(),don't(),mul-+[where()$,mul(238,155)}(&amp;&lt;&gt;;[!do()where()(mul(246,69)?from()where()!mul(385,209)who())&lt;(when()!,[;mul(567@&lt;})&gt;mul(214,524)}#%&gt;[mul(429,28) who(){from(664,943)&gt;?mul(747,239)+!!who(75,291)(where()&amp;from()mul(363,660)why()~mul(971,115)when()what()where()']do()/#/;&lt;+)mul(313,612)(why()@&lt;mul(886,716)&gt;[why()#from()where()how()^where(929,904)@do()*from(936,438)[ when()+:mul(772,586]*mul(843,866)&lt;}+[/&amp;^-when()mul(62,918)[mul(602,984)&amp;@~where()how()^when()&gt;'/mul(3,2)&lt;]mul(134,654)&lt;-};mul(456,534)/({ what()do();,*select()]^)mul(528,106)&lt;&gt;mul(157,393)  &amp;where()mul(697,508)mul(793,680)+[&lt;mul(176,69),-}-']how()@+mul(311,266))mul(771,898)from()+why()mul(441,294)$&gt;?%$~~%don't()mul(882,564)mul(954,646)]&amp;%how()mul(322,840)~select()mul(589,361);#!&lt;mul(617,898)/@&lt;when()'mul(118,907),mul(140,382)&amp;@$^select()$when(617,295);do()&amp;$&lt;^&amp;when()+*mul(132,674)^]/(:;}*}/do()@':' mul(900,79)/select())][mul(238,573)-what()how(){)@%$-;mul(266,561)when()@:!'mul(150,805)&gt;#mul(781,972)mul(764,49)*?^}where()mul(698,69)]&lt;&amp;(what()[^&lt;&amp;mul(438,77)?@who()who()when()mul(712,314))^? mul(806,50)]},@(mul(522,258))mul(750,831)^mul(2,167)where()@@what()[)select()mul(480,518); ^&amp;how()%]mul(856,366)select()}when()/]!#?%where()mul(246,951)~why()&amp;%/{^mul(771,634)# {how()when()&gt;+#![mul(489,260)!::?'&lt;how()&amp;&gt;from()mul(527,396)&amp;})mul(557,921)$&gt;[!mul(551,664)&gt;[mul(868,16)}:how()how()^;/mul(641,963) {mul(130,436)&gt;~?&lt;@+]mul(745,360):)[/?]@mul(796,631)where())why()~~mul(191,523)how()mul(902,53)-what()where()who()!from()mul(908,532)who()how():${@#mul(998,383)$,[:;mul(154,723)]]+ &amp;%&lt;],mul(279,823)&lt;when()who()]]don't()&lt;; ]%[what()mul(55,665)$from()from()' mul(412,420),-[where()from()mul(853,815)/from()&lt;*^&gt;&lt;mul(379,392)why()&gt;{who()mul(171,633)&amp;^when()&lt;mul(881,444),select()/-&lt;[^@ !mul(547,699)}' when(201,621)mul(147,38)$where() ~how()${do(){&lt;mul(185,208)}[[mul(596,100)what()why()![?don't()%(;mul(827,857)^from(),who())}mul(114,321);^from()&amp;)$^mul(889,568):why()~!*mul(775,388)^where()/mul(90,546)&lt;#}[what()&gt;&lt;}'from()mul(408,866)select()#how()?mul(818,40)where():$)when()[&amp;who())mul(203,389){why(717,710)where()$}])~how()mul(608,627))how()where()$-why()/mul(296,533){mul(341,534));$#/&lt;mul(858,725)[where()}:from();when()&amp;mul(703,386)where()from()#^how()&amp;&gt;-^mul(501,854)^^+&gt;what()]how()*:+mul(69,163)*;mul(810,823)-when()/)(mul(825,165)what()&gt;])~@/mul(495,234)?] mul(918,879)]^';%)when()#?mul(656,686)*;&lt;where();mul(461,612) @when()what()[('what()mul(838,164)@}/;~mul(96,648);!{&lt;])~mul(817,690)select()*~select()(why())}mul(7,265)(]mul(459,756)mul(909,698)&amp;-do()$where()%~-~mul(622,257)select()where()*!(mul(764,419)?()*when()}</t>
   </si>
   <si>
-    <t>find )</t>
+    <t>Input</t>
   </si>
   <si>
-    <t xml:space="preserve"> (who() what())&gt;when()why()'mul(454,153)mul(565,994)(mul(890,533)#mul(875,768)+'-^where()}when()mul(103,598)[mul(401,600)when()from()how()+mul(928,225)why():mul(909,344)when()'?where():(what()mul(972,219)${/ mul(402,908)who()&amp;where()~where()mul(60,961)#]$mul(459,473))})~mul(143,89),select()mul(772,463)mul(742,92)&lt;(]},select()[%^when()don't()select()from()mul(776,917)+!!why()when(485,399)what(720,754)from()&amp;mul(746,260)where()*who()~&amp;/from()what()]what()mul(694,820)%why(16,195)when()'why() [when()why():do()when(),'&lt;?{who()mul(296,514)%mul(442,333)when()-,why()[!:+from()mul(774,695)}where()*-!%mul(834,493){-&amp;(??mul(240,739)from()@@}@mul(796,837)[;mul(301,618)mul(933,68)+%}/$&lt;mul(879,769)'&amp;('#-mul(314,537);who()where(134,686) where(975,359){how(900,557)mul(134,21)when() !*!$^mul(670,298)*!}:-how(429,820)~]mul(414,322)-select()?what()when()]&gt;#from()(mul(200,440)/]mul(58,834)@&lt;select()mul(966,435)&lt;+;mul(98,983)&lt;;,;how()&amp;'@mul(727,703)!?&gt;!!mul(175,542)mul(363,28)]}don't()+[{&lt;@/,mul(103,154)mul(808,942)$where()why()from()[mul(780,395)^why()#-!:~why()+mul(879,633)&lt;[where()!what()-,mul(6,80)how()?)^select()&lt;}when()]how()mul(385,345)~?don't()&lt;)'mul(557,404)+;/&lt;;}%?//mul(586,270);^&amp;,^}'&amp;:mul(914,485)&gt;,$mul(616,138)'[/-mul(786,357)&amp;why()where(490,893)/-}*}mul(967,485)!'mul(664,982),when()^why()$%(,why()mul(826,970)$*~'),+when()-mul(586,837)+;(/%{[what(201,897)mul(540,583)don't()}mul(358,207)mul(988,94)$#&amp;&lt;?+why()mul(82,18):from()select()!~mul(805,768)&amp;+! how()what()?select())mul(779,277)[&gt;}mul(580,42)#select(190,243){*%*from()mul(491,435)* mul(345,720)+#{)/,'&lt;},mul(529,664)? don't()'mul(925,474)}:!?]mul(655,353)when()'how()(don't()how()^/where())select()select()^~{mul(39,73)['[&lt;^)/!;&lt;mul(367,290)$select()when()^when()&gt;mul(338,323) ~* who()what()where()mul(746,703)mul(70,40);/&lt;select()mul(557,879)*&gt;:!mul(89,464)when()how()~?;~}mul(669,359)+mul(64,989)why()what()where(478,19)^from()$mul(49,43):why()mul(946,368)who()%?{'why()mul(754,618)select()}^mul(925,787)how()select()&lt;^;{}}%mul(857,178)@?$;)%what()['mul(343[&lt;^mul(622,524)$#{&amp;where();@how() #mul(572,8)who(244,369)/*;;mul(22,910)how()?who(200,683)#what()why()mul(9,541)don't() %&gt;mul(583,678)mul(977,618)mul(846,566):@mul(601,58)%mul(12,677)^#[how()?do()&amp;'%how(985,614);@? 'mul(295,467)}@mul(462,179)[from(946,303)@what(236,293),from(572,15)^mul(602,286/*:(select()!mul(950,26){^}]-mul(541,949){/select() from(202,590)what()]select()~mul(931,833)^/}where()*mul(665,272)*'where()&gt;} :]mul(470,26))mul(945,496)%-!;-* mul(958,735)+mul(292,844)where()mul(323,887)select()how()why()%~why(974,789){!/:mul(890,844)&amp;]{'mul(727,812)?mul(521,348)']~,mul(604#what(201,469)]{'how()#[mul(68,187){#+%* when()+when()mul(270,65)select())how();! %where()]@mul(267,348)from()select()who(579,714)where()mul(359,887why()who(120,403)from()&amp;!)do()mul(614,872)select()[:who()'&gt;&gt;?]who()mul(373!:&gt;&amp;mul(13,848)~how()who()+*what()&amp;mul(214,262)/where(941,723)mul(34,526){ }( ~from()){ mul(648,400)mul(946,270)where()&lt;mul(672,282)&amp;'&gt;,mul(156,431)when(444,909)mul(10,765)#mul(393,855)how()@&amp;from()mul(538,109)[%^-&lt;(how()}how()mul(841,917)~ ]^! ^select()mul(624,87))what()&amp;[-'/&amp;)mul(113+from()how()why()]&amp;&gt;mul(82,319)&amp;:''where()/&lt;;mul(882,75)&gt;/^#/how()!mul(481,243)}*!what()#}#mul(93,825)&gt;'(!where()(&amp;mul(417,293)&gt;[{*()}how(349,243))mul(577,515)}mul(644,588)why()~~what()'why(658,231)]where()mul(260,870)mul(82,64)$+&gt;,&amp;$where()$why()where()mul(513,597),when()why()&amp;mul(559,679/why();~{mul(876,302)/+why(921,489);%@from(){do()&amp;+from()mul(646,666)how() }^;{!?mul?),$*mul(244,591)&lt;)select()(&lt;where()(!mul(708,996)/*@;;:mul(760,261)when(338,104)mul(870,299)!}(mul(269,625) who(553,681)&amp;mul}[#{who()%what(){,when()mul(723,486)-/?{mul(475,745)&amp;%select()%'who()&lt;?:mul(117,765):{&gt;^select()where(454,602)when(){mul(201,421)) ,when()$/$;#;mul(715,512)~-mul(110select())&amp;/;&gt;:^')+mul(525,861)mul(94,520)select();mul(200,362)mul(662,110)what()[';mul(706,110)mul(524,196{ from()%/from()when()select()*mul(952,760)@&lt;@(mul(359,289:?[!:mul(788,331)&gt;(-mul(790,172)~/';(#mul(744,504)}@!#:!)where()mul!why()&lt;+mul(24,595)($/why()&amp;(&lt;mul(872,460%where()[who()mul(962,669):&lt;+-from()]mul(454,164)-,what()@+'mul(10,853)-@@){}what()mul(909,997) ^why()@!/from()$]mul(97,897)?mul(935,220)why()[:*)^) #/mul(301,584)@where()how()mul(609,313)':mul(949from();who())who()who()mul(491,372)!&gt;&gt;'why()}/mul(809,414)mul(202,168)&amp; where(){- ]where()where()&lt;mul(281,296);&amp;mul(625,586)!/{]&amp;+&gt;who()&gt;^mul(543,106){don't():/('why()when()[):#mul(261,544)why()-+mul(325,976)-why()&amp; what()who()%*&amp;;mul(309,586)from()~;mul(527,332)]how()when()mul(266,71)mul(383,68)how()from()}how()[{;who()why()mul(479,649)-who()&gt;mul(954,835))(,'?)why(),mul(73,982)-+mul(275,963)?:*&gt;+%%}%mul(159,868)[{mul(849,590)where()how()when()mul(380,542),'{mul(716,261)@$what()[where(961,898)+#;mul(102,332))mul(151,993)who(433,641)what()!],{&lt;why()#mul(449,110)?from()~how()how()how(425,48)where()~mulwhen()mul(427,877)when()+!&lt;who(),&gt;}mul(225,989)from()$&gt;'/&gt;mul(271,482)(]when(703,790)$['&amp;don't()^ mul(292,747)why();;from()why() #[??mul(675,831)*/&lt;{when()%mul(82,353)?~(~@from()-mul/,when()[+', /why()mul(531,95)')&lt;&amp;#]#!&lt;mul(172,129)mul(543,657-[&lt;,:,:@mul(458,222)mul(640,872)^mul(45,292)!&amp;#+mul(859,346)[:+^$how()(&lt;when()mul(247,266)mul(468,925)&amp;select()^who()~))mul(184,981)from() when()+select()&gt;where()&lt;when()mul(420,131)+-select(379,472)-$from())mul(402,68)what()#mul(278,846)#who()~)?mul(287,731)-- mul(989,728)#$when():mul(470,964why()$ )-?,':from()from()mul(54,842)}mul(581,400),{$select()select()how()mul(531##mul(272,787)['{(don't(),[how()?@where()@-^-mul(55,325)#,][?mul(437,664)+-select()what():/%'mul(569,297))'?/*{mul(40,581)^how()where()!who()#[mul(828,836)$why(819,535)who()#/&gt;$&gt;select()[mul(326,511)/:#::when()(do();mul(960,765$mul(947,618)!from(704,544)-);select()}mul(278,843)&amp;+-&amp;)!}select()why()mul(333,183)!~mul(360,636)}@mul(43,235)&amp; ~*how()~&amp;&gt;$~mul(163,420);@' mul(328,120)&amp;}#)what()~[~!mul(892,685);from())*select()]from(),mul(454,194)!what(598,913)~what()who()*),*who()mul(651,343)~'mul(311,104)~%~how(){when(){mul(348,414)!who()when(),mul(565,187)'who()mul(573,606)/]&lt;why())mul(29,128)%from()select();]where()'%mul(515,513):'why()/&lt;&amp;#%-mul(54,420)what()mul(253,192)}how()+mul(344,599[$who()#what()@from(850,461)mul(670,417)why()!mul(77,694)who()::+who()(^mul(580,475)(&gt;/?^{do()when(),mul(301,391)select()!]%mul(662,532)why():&gt;mul(317,266)-]/!#?~what(395,165)mul(882,259)(how(){%)from(355,754)from(){?+mul(251,179)+}$^-[mul(244,700), $$mul(989,641)how()&amp;&gt;[{(@when()!mul(17,250)why()mul(516,948)/from()&amp;)](~who(),mul(936,726)from()who()mul(642,108){?/*&lt;mul(421,307) mul(954,385)@-who()-]why()do()mul(152,214)?)what()what() ){select()/mul(88,987)(&amp;;^where(687,768)mul(592,288)&gt;:who()](-)[mul(234,936)//select(){don't()}!mul(711,979)when()why()~( what()%from()^:mul(970,839)who()~$from()how()mul(525,184)(*}from())mul(592,712)select()where()from()do()/!from()@%* /:mul(796,770)[select()mul(737,95)*who()mul(538,295)from()when()mul(202,997)mul(920,622)[^,'^{~&amp;mul(890,310)-#mul##$what()how(),*{]what()'mul(753,51)why()from()%+*-mul(44,560)^/who() how()mul(846,745),$ mul(884,965)?];@;'mul(607,810)]don't()?mul(15,474)*^%where()&gt;,#- mul(381,876)&gt;]'how()[]?when()mul(350,528)&amp;&gt;%%#*;mul(465,783)?/from()'mul(109,659)*'mul(260,549))where(427,3)mul(750,184)mul(514,568)+ &lt;mul(142,867)do(){ mul(197,631)*[~![mul(592,975)&gt;where(838,713) ~$]{what()mul(505,954)&lt;&gt;;-#:mulwhat()[!]why()mul(899,266)%}&gt;select()?]'mul(936,764),~mul(189,689)}^mul(474,190)&lt;;&amp;&gt;]how()/{mul(271,843)&gt;}why(522,791)what()do()#/^where()%when()!mul(284,340)##[why() when()&gt;{mul(998,539)*[*):'&gt;'mul(577,914)[*)who()mul(305,505)who()!@how()'}when()mul(331,543))mul(91,478)(where(196,348)&amp;:]&gt;?mul(560,724)where(872,560)&lt;% what()*where()]select()do()(what()-~mul(229,896){?~when()mul(826,622)&amp;(#mul(451,442))what()mul(866,906)how()$-&amp;where()&gt;-([mul(199,824)!~)$/&lt;:mul(727,123)do()$*-#-@+where()select()$mul(612,415)who()$#,who()&gt;/from()mul(967*who();%@}how()/why()}mul(106,998)how():(;&amp;mul(345,702)mul(275,94)]#&gt;{mul(426,479)why()&lt;;~what()$!+@'mul(40,71)&amp;when()*%mul(973,215),what(),mul(709,788)who()):mul(205,236)~mul(50,81)+how()%~/mul(748,800)(}}mul(124,528)mul(129,959)%[&amp;[select()mul(547,292);who()&gt;???why()+who()mul(442,582):how()&gt;select(92,760);+mul(440,501)@/@&gt;#&amp;:mul(764,753select()%:how()where(202,288) mul(613,367)how()?mulselect(255,7);[;why()/$ mul(351,228){mul(312]+!^#+,why()what(327,951)mul(134,668)&amp;&lt;why(575,717) $-('mul(810,445),mul(731,60)^:mul(695,596)~*^;/mul(570,879)why()where()where() select()what();(from()&lt;mul(11~what()select()how()$-&lt;%mul(335,108)~[)mul(759,937)mul(93,397)when()&gt;&amp;?'!why()where()mul(172,288)+mul(90,27):';*@how()/what()mul(272,960)select(845,387)don't()&lt;select(142,144)how(){}mul(525,125)mul(513,731)from()@,@}why():;:don't()+why()mul(758,764)@,:mul(248,570)/!mul(352,81)what()/?&lt;::what(),}^mul(723,61)'$'^don't()!-from()$**^mul(340,35)where()why(16,588):-mul(895,416)$how()!where()'~{'+,mul@where()&lt;(who():&lt;mul(857,771)}mul(231 when())+mul(494,721)#!/usr/bin/perlmul(361,116)(^*mul(552,797)mul(235,864)[%@~}~mul(222,585))where()where()/{^#@mul(3,798)what()what()where()why()#how()&amp;mul(607!who()+select()what(315,999)/mul(322,478)'when(),why(885,556)select(747,859)^}how()#mul(994,4)what()&lt;/(mul(534,885)who())};from()why()}from()~what()mul(858,35!:why()what()what()mul(716,993)why()&gt;}--}}?)mul(509,779)-)mul(682,498))from()#mul(69,525)%-?&gt;&gt;mul(68,359)/mul(923,989from()~mul(132,353)mul(980,998) (where()}*&gt;&amp;how()[mul(570,289)*~mul(388,859)how(829,278)[&lt;]who();&lt;who()[mul(833,723;mul(208,875)&gt;mul(199,174)*~:[what()^}#who()&gt;mul(221,636)*-()%-when()from()mul&amp;}who()[mul(725,983)&gt;#!who(592,5)%mul(85,978)what()'mul(178,305)[[?:#-&gt;#! mul(374,804)&lt;$&amp;{-&gt;++mul(446,37)-#&amp;}%)mul(19,914who()(# ;mul(959,330)what()&gt;#who()who();mul(228,273)from()+}/&amp;why(783,754)from()(#mul(649,849)*why(){why()(who()?!why()from()mul(344,447):how()+when(144,750)what()mul(217,542)where())%mul(253,8),$how()%[&gt;#from(),:mul(174,127)-:when()-don't()where()(when()&amp; ]^from()mul(263,164)mul(873,530)::@select()mul(459,547)why()!}$*mul(674,506)&lt;mul(665,313)@mul(310,284)when()how()#;+({@~mul(655,423)(?where(868,382)where()@mul(190,467))-when()~how()mul(71,646)where()how() mul(362,510)&gt;*]~don't()mul(570,150)what()do()&lt;'^)~mul$mul(508,426)/why()mul(155,774)~?from()![mul(670,674)select()?^when()from()]{mul(736,574){&gt;'~^mul(248,37where()@:where(938,730)select()!'&gt;,;mul(827,796):what()%where()!/how(231,307)mul(88,489)@!!mul(173,890)how()[- +what()+$~mul(244,436)(why(),[,-;[&lt;%mul(991,950)%mul(804,561)&amp;:,mul(442,575)}~what(523,563)?+ how()/}[mul(866,343)]:where()where()&gt;$mul(423,440)~&gt;[mul(259,864))@ {^mul(256,238)[:]*$$mul(206,916)*}!what(937,263)select()}don't()'*&amp;mul(630,249),mul(521,101)&lt;where()?where()how()from()select()&lt;when():mul(185,154)$*&lt;(do()]{mul(231,307)$*@* why()select()%'@mul(564,503)@ !@mul(245,476)who()how()$@~select()&gt;/who()!mul(884%/&amp;;^from()mul(846,533);}why()?;mul(538,765)+,([ !}@]{mul(98,545) ~how(703,291)]#)~[[mul(588,167)*-+mul(246,51);+from(){;;what()/:?mul(921,460)&lt;@where()mul(674,502)/)select()%~what()?)mul(406,916)&gt;/mul(501,656)]mul(979,533)/why()*select()where(),^mul(370,549)^~how()why()+,how()@mul(168,884)',&lt;$]mul(377,183)+$&lt;mul(48,619)who(625,236)who()#where()}mul(43,845)why()(?~mul(575,269)&amp;who()why()(!where()-]mul(482,691)where(745,121)from()^/{mul(784,137)@where()(#do():-%]''{mul(901,539)/@who()%&lt;mul(979,206)mul(705,493))&gt;mul(425,602)when()~'&gt;when(),when()%mul(231,25)[why();'!mul(879,941/who()mul(658,479)why()where()*mulwhen()mul(486,551)where()?,)~ what(221,542)/;mul(260*how()~~why()mul(571,395)mul(319,33)where()mul(313,612)select(458,89)when()?from(),)[%^[mul(489,554){mul(482,42)from();mul(911,838)from()what()&amp;/when()when()mul(748,509)/!&amp;who()mul(98,104)what()',how(660,701)^mul(904,678)&amp;}'mul(498,173select()% -from()!when()mul(918,395)?&lt;&lt;@mulhow()/from()][don't()+select()who()what():^^@mul(826,867)select()^[@mul(673,493)select()@(select()mul(152,937),why(955,595)select()where()-'mulwhere()~?mul(572,408)when(606,22){~*(mul(971,805),how(402,696)')}who()&amp;@*who()mul(76,96){where()mul(711,3)*-+~where()mul(812,534[select()!#(how()mul(799,474)&gt;mul(251,649)(from()what();-do()~;]what(),what(393,86)?mul(892,224)who()mul(635,260)mul(300,39)}&gt;select()&gt;@why(364,672)who():where()mul(385who()))&gt;when()why()&amp;&gt;mul(276,702)&amp;:mul(192,782)/:)@mul(948,155)[!don't())what(),what()mul(747,717)#?$mul(967,489)when()who()why()#mul(961,811)what()mul(307,623)~}from()how(),mul(669,93)^ &amp;select()how()mul(105,129)?])*)mul(246,433):)how()mul(941,140)&lt;[ ;&amp;*mul(580,48);%%'why()what()( %mul(189,229)]'&lt;@)/mul(741,684)[mul(632,558)'@what()what()mul(986,227)&lt;how(584,802)$mul(698)@;+%+;mul(704,986){{how()where()what()from()where()$do()where()why()*-mul(752,877);where()//*?*&gt;&lt;?mul(33,338)where()where()[&gt;select()/from()*when()@mul(747,356)mul(674,720)mul(10,513))]#]-mulwhat()select(501,639)mul(114,558)[}$]who()mul(759,134)#who()/@*mul(444,475)!@+don't()#when()}where()[where()',select(){mul(206,80)/&lt;what(230,519)-mul(424,213)&gt;!&amp;how()+]^mul(847,293)+(mul(837,220)/!#!mul(613,470)&lt;mul(93,129)who()from()&gt;#where()from()&amp;$mul(29,370how()]&amp;&lt;where()from(283,113)mul(336,151)select();-from()'why()when()how()(what()mul(467,47){{??mul(513,543);)mul(397,402)mul(428,472)who()~{mul(262,609)how()from(){'  /who()select()mul(778,88)~&gt;/-where()%from())&gt; mul(251,617)-why()~^don't()##~mul(176,935)[;%@?^,don't()!mul(564,493-(&amp;+@'[&lt;*;mul(241,470)&lt;&gt;}mul(684,534):?&lt;do()mul(336,113)&gt;[&gt;?+:mul(835,881)mul(901,992)mul(595,306what()% mul(333,684),what(910,959);^what(),where()'mul(493,314)}-what()&amp;who(231,428)where()&gt;' &lt;mul(754,558)how()+what(734,212)]how()$)^mul(991,39))-'}{mul(459,367);@^-?]?$?mul(32,624)how())mul(741,402)*@]when()mul(559,247)when()don't()((,[}-why(692,780)({{mul(788,419)how() -)mul(710,838)mul(952,75)/!#')[([&lt;mul(547,553)(@&lt;!~]#+who()+mul(597,266)&gt;[where(),]who()mul(215,607)&amp;'mul}select()^%&lt;!mul(523,490);';)(@}&gt;/what()do()&amp;mul(735,766)#%$']*;/+do()~what()how();$#[/select()mul(73,86),who()#who()?*&lt;mul(285,423)'@don't()-!$};where()^%mul(846,592)mul(129,272)[)&lt;when()&gt;[mul(839,173)&amp;$$[why(349,377){why()&gt;why()mul(49,44)@'};!)*;mul(265,467)why()}'mul(561,416)}]-mul(334,113)mul(126,247)}mul(536,247){?mul(780,762)&lt;from()~-] @+$mul(416,370)$mul(617,551)who(647,22){&lt;':}!when()how()mul(541#what())~select()where(257,55)?when(446,792)mul(654,34)mul(30,36)^+'}*mul(835,84};)mul(348,922)who()what(424,481))$(!@^[mul(934,712[&gt;,how()&lt;'who()what()%&lt;?mul(909,44)how()~(do()[&lt;]+[mul(30,114)select()where()[&gt;what()mul(324,650)* ^)mul(116,480)&amp;  %&gt;,mul(722,539)-who()mul(69,643))+select()&lt;'mul(398,585)mul(635,160),!{}mul(218,149))(why()[when(),mul(4,152)@what()*@&gt;@how()mul(78,645)@*#}#select()({mul(196,97)when()@what()+why(287,586)when(){mul(908,484{%-where(){'from()mul(254,416)how()}*(how()#@}mul(670,932)mul(741,232)&amp;'!?@$mul(775,804);),,!mul(757,128)/?'!mul(47,297) $/,,:@~select()?mul(604,497);mul(770,711)+mul?where()/mul(777,175)^&gt;where()&lt;#mul(376,176)~){}mul(758,497)!){%where(), mul(360,122,mul(54,973)):mul(248,44)[where()^mul(162,809))*what()^?+}what()how()why()mul(839,131)mul(913,94) why(),why()'mul(459,43)&lt;-from(),#%{]%/mul(733,345){,/+&lt;[?mul(292,416)&amp; [&gt;/^why(408,559)mul(648,879)#)$ +how()where()#mul(708,178)how()*[mul(560,727)*when()from(); &gt;~]'&amp;mul(90,393)$~from()mul(578,828)mul(710,50)?+@what()@+!;mul(250,79)when())'mul(523,730)+*}^*mul(698,766)&lt;-why()-/:!/select(),don't(),mul-+[where()$,mul(238,155)}(&amp;&lt;&gt;;[!do()where()(mul(246,69)?from()where()!mul(385,209)who())&lt;(when()!,[;mul(567@&lt;})&gt;mul(214,524)}#%&gt;[mul(429,28) who(){from(664,943)&gt;?mul(747,239)+!!who(75,291)(where()&amp;from()mul(363,660)why()~mul(971,115)when()what()where()']do()/#/;&lt;+)mul(313,612)(why()@&lt;mul(886,716)&gt;[why()#from()where()how()^where(929,904)@do()*from(936,438)[ when()+:mul(772,586]*mul(843,866)&lt;}+[/&amp;^-when()mul(62,918)[mul(602,984)&amp;@~where()how()^when()&gt;'/mul(3,2)&lt;]mul(134,654)&lt;-};mul(456,534)/({ what()do();,*select()]^)mul(528,106)&lt;&gt;mul(157,393)  &amp;where()mul(697,508)mul(793,680)+[&lt;mul(176,69),-}-']how()@+mul(311,266))mul(771,898)from()+why()mul(441,294)$&gt;?%$~~%don't()mul(882,564)mul(954,646)]&amp;%how()mul(322,840)~select()mul(589,361);#!&lt;mul(617,898)/@&lt;when()'mul(118,907),mul(140,382)&amp;@$^select()$when(617,295);do()&amp;$&lt;^&amp;when()+*mul(132,674)^]/(:;}*}/do()@':' mul(900,79)/select())][mul(238,573)-what()how(){)@%$-;mul(266,561)when()@:!'mul(150,805)&gt;#mul(781,972)mul(764,49)*?^}where()mul(698,69)]&lt;&amp;(what()[^&lt;&amp;mul(438,77)?@who()who()when()mul(712,314))^? mul(806,50)]},@(mul(522,258))mul(750,831)^mul(2,167)where()@@what()[)select()mul(480,518); ^&amp;how()%]mul(856,366)select()}when()/]!#?%where()mul(246,951)~why()&amp;%/{^mul(771,634)# {how()when()&gt;+#![mul(489,260)!::?'&lt;how()&amp;&gt;from()mul(527,396)&amp;})mul(557,921)$&gt;[!mul(551,664)&gt;[mul(868,16)}:how()how()^;/mul(641,963) {mul(130,436)&gt;~?&lt;@+]mul(745,360):)[/?]@mul(796,631)where())why()~~mul(191,523)how()mul(902,53)-what()where()who()!from()mul(908,532)who()how():${@#mul(998,383)$,[:;mul(154,723)]]+ &amp;%&lt;],mul(279,823)&lt;when()who()]]don't()&lt;; ]%[what()mul(55,665)$from()from()' mul(412,420),-[where()from()mul(853,815)/from()&lt;*^&gt;&lt;mul(379,392)why()&gt;{who()mul(171,633)&amp;^when()&lt;mul(881,444),select()/-&lt;[^@ !mul(547,699)}' when(201,621)mul(147,38)$where() ~how()${do(){&lt;mul(185,208)}[[mul(596,100)what()why()![?don't()%(;mul(827,857)^from(),who())}mul(114,321);^from()&amp;)$^mul(889,568):why()~!*mul(775,388)^where()/mul(90,546)&lt;#}[what()&gt;&lt;}'from()mul(408,866)select()#how()?mul(818,40)where():$)when()[&amp;who())mul(203,389){why(717,710)where()$}])~how()mul(608,627))how()where()$-why()/mul(296,533){mul(341,534));$#/&lt;mul(858,725)[where()}:from();when()&amp;mul(703,386)where()from()#^how()&amp;&gt;-^mul(501,854)^^+&gt;what()]how()*:+mul(69,163)*;mul(810,823)-when()/)(mul(825,165)what()&gt;])~@/mul(495,234)?] mul(918,879)]^';%)when()#?mul(656,686)*;&lt;where();mul(461,612) @when()what()[('what()mul(838,164)@}/;~mul(96,648);!{&lt;])~mul(817,690)select()*~select()(why())}mul(7,265)(]mul(459,756)mul(909,698)&amp;-do()$where()%~-~mul(622,257)select()where()*!(mul(764,419)?()*when()}</t>
+    <t>Regex extract</t>
+  </si>
+  <si>
+    <t>Index of ','</t>
+  </si>
+  <si>
+    <t>Index of ')'</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>sum</t>
   </si>
 </sst>
 </file>
@@ -146,10 +164,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -472,7 +486,7 @@
   <dimension ref="A1:H666"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,16 +498,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="str" cm="1">
         <f t="array" ref="B2:B666">_xlfn._xlws.PY(0,0,A2)</f>

</xml_diff>